<commit_message>
Maps of glm predicted vs. observed
</commit_message>
<xml_diff>
--- a/GLM/glm summary 9-11-2014.xlsx
+++ b/GLM/glm summary 9-11-2014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="10110" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="23820" windowHeight="10110" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="2" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="model.avg" sheetId="1" r:id="rId4"/>
     <sheet name="table for comparison" sheetId="3" r:id="rId5"/>
     <sheet name="summ_responses" sheetId="4" r:id="rId6"/>
+    <sheet name="confusion_matrix" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="174">
   <si>
     <t>Estimate</t>
   </si>
@@ -1319,6 +1320,35 @@
 dist_LM (+)
 secchi (-)
 lakes_1km (-)</t>
+  </si>
+  <si>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>Present</t>
+  </si>
+  <si>
+    <t>Observed</t>
+  </si>
+  <si>
+    <t>Predicted</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wolffia </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sp.</t>
+    </r>
+  </si>
+  <si>
+    <t>Floating plant presence</t>
   </si>
 </sst>
 </file>
@@ -1700,7 +1730,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1839,6 +1869,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1884,7 +1923,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1964,12 +2003,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1992,6 +2025,23 @@
     <xf numFmtId="166" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3243,8 +3293,8 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6116,8 +6166,8 @@
   </sheetPr>
   <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6136,19 +6186,19 @@
       <c r="A1" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="49" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6159,11 +6209,11 @@
       <c r="B2" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
     </row>
     <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
@@ -6271,19 +6321,19 @@
         <v>19</v>
       </c>
       <c r="B8" s="26"/>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="F8" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="49" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6294,11 +6344,11 @@
       <c r="B9" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
@@ -6406,19 +6456,19 @@
         <v>149</v>
       </c>
       <c r="B15" s="26"/>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="E15" s="41" t="s">
+      <c r="E15" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="F15" s="41" t="s">
+      <c r="F15" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="49" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6429,11 +6479,11 @@
       <c r="B16" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
@@ -6541,19 +6591,19 @@
         <v>150</v>
       </c>
       <c r="B22" s="24"/>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="41" t="s">
+      <c r="D22" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="E22" s="41" t="s">
+      <c r="E22" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G22" s="41" t="s">
+      <c r="G22" s="49" t="s">
         <v>97</v>
       </c>
       <c r="I22"/>
@@ -6580,11 +6630,11 @@
       <c r="B23" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
     </row>
     <row r="24" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="26" t="s">
@@ -6692,19 +6742,19 @@
         <v>151</v>
       </c>
       <c r="B29" s="30"/>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="41" t="s">
+      <c r="D29" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="E29" s="41" t="s">
+      <c r="E29" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="F29" s="41" t="s">
+      <c r="F29" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G29" s="41" t="s">
+      <c r="G29" s="49" t="s">
         <v>97</v>
       </c>
     </row>
@@ -6715,11 +6765,11 @@
       <c r="B30" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
     </row>
     <row r="31" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="26" t="s">
@@ -6860,31 +6910,31 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="D29:D30"/>
     <mergeCell ref="E29:E30"/>
     <mergeCell ref="F29:F30"/>
     <mergeCell ref="G29:G30"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="84" orientation="portrait" r:id="rId1"/>
@@ -6895,8 +6945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="A1:C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6907,68 +6957,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="42" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="49">
+      <c r="C2" s="47">
         <v>27.1</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="C3" s="49">
+      <c r="C3" s="47">
         <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="44" t="s">
         <v>166</v>
       </c>
-      <c r="C4" s="49">
+      <c r="C4" s="47">
         <v>14.3</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="44" t="s">
         <v>163</v>
       </c>
-      <c r="C5" s="50">
+      <c r="C5" s="48">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="44" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="47">
         <v>30.9</v>
       </c>
     </row>
@@ -6976,4 +7026,234 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C2" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="52"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="51"/>
+      <c r="C3" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="53" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="54">
+        <v>104</v>
+      </c>
+      <c r="D4" s="54">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="53"/>
+      <c r="B5" s="51" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="54">
+        <v>14</v>
+      </c>
+      <c r="D5" s="54">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="52"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="21"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="53" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="54">
+        <v>143</v>
+      </c>
+      <c r="D10" s="54">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="53"/>
+      <c r="B11" s="51" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="54">
+        <v>0</v>
+      </c>
+      <c r="D11" s="54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="55" t="s">
+        <v>172</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14" s="52"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="21"/>
+      <c r="C15" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="53" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="54">
+        <v>150</v>
+      </c>
+      <c r="D16" s="54">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="53"/>
+      <c r="B17" s="51" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" s="54">
+        <v>1</v>
+      </c>
+      <c r="D17" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="52"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="D21" s="51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="53" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" s="54">
+        <v>82</v>
+      </c>
+      <c r="D22" s="54">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="53"/>
+      <c r="B23" s="51" t="s">
+        <v>169</v>
+      </c>
+      <c r="C23" s="54">
+        <v>20</v>
+      </c>
+      <c r="D23" s="54">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A10:A11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>